<commit_message>
Updated Excel files with primary track settings.
The GT+ST and allGT+allST configurations are no longer identical to GT and
allGT.

Signed-off-by: Klas Magnusson <klasmagnus@gmail.com>
</commit_message>
<xml_diff>
--- a/Settings-GT+ST.xlsx
+++ b/Settings-GT+ST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\BaxterAlgorithms_CSC2019\CTC_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB923936-0403-4DB5-91B8-78ABC3FB23B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B6ED5F4-5DFC-4F38-AEB0-14B3CDD166A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="31260" yWindow="2430" windowWidth="21600" windowHeight="12735"/>
   </bookViews>
   <sheets>
     <sheet name="Settings-GT+ST" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="135">
   <si>
     <t>setting</t>
   </si>
@@ -55,355 +55,376 @@
     <t>BF-C2DL-HSC</t>
   </si>
   <si>
-    <t>3.1839</t>
-  </si>
-  <si>
-    <t>1.468</t>
-  </si>
-  <si>
-    <t>0.69319</t>
-  </si>
-  <si>
-    <t>0.082824</t>
-  </si>
-  <si>
-    <t>0.56165</t>
-  </si>
-  <si>
-    <t>0.0315</t>
-  </si>
-  <si>
-    <t>58.6413</t>
-  </si>
-  <si>
-    <t>134.3994</t>
-  </si>
-  <si>
-    <t>43.3024</t>
+    <t>3.9162</t>
+  </si>
+  <si>
+    <t>1.6455</t>
+  </si>
+  <si>
+    <t>0.60878</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.53142</t>
+  </si>
+  <si>
+    <t>0.037518</t>
+  </si>
+  <si>
+    <t>85.913</t>
+  </si>
+  <si>
+    <t>130.6222</t>
+  </si>
+  <si>
+    <t>40.9816</t>
   </si>
   <si>
     <t>BF-C2DL-MuSC</t>
   </si>
   <si>
-    <t>4.5649</t>
-  </si>
-  <si>
-    <t>3.2892</t>
-  </si>
-  <si>
-    <t>0.88394</t>
-  </si>
-  <si>
-    <t>0.70291</t>
-  </si>
-  <si>
-    <t>0.01699</t>
-  </si>
-  <si>
-    <t>5.8063</t>
-  </si>
-  <si>
-    <t>50.3551</t>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>3.75</t>
+  </si>
+  <si>
+    <t>0.942</t>
+  </si>
+  <si>
+    <t>0.0014611</t>
+  </si>
+  <si>
+    <t>0.63028</t>
+  </si>
+  <si>
+    <t>0.012114</t>
+  </si>
+  <si>
+    <t>2.159</t>
+  </si>
+  <si>
+    <t>213.1184</t>
+  </si>
+  <si>
+    <t>68.3584</t>
   </si>
   <si>
     <t>DIC-C2DH-HeLa</t>
   </si>
   <si>
-    <t>4.3124</t>
-  </si>
-  <si>
-    <t>3.7263</t>
-  </si>
-  <si>
-    <t>0.24872</t>
-  </si>
-  <si>
-    <t>0.20081</t>
-  </si>
-  <si>
-    <t>0.020217</t>
-  </si>
-  <si>
-    <t>4.4662</t>
-  </si>
-  <si>
-    <t>2209.0181</t>
-  </si>
-  <si>
-    <t>752.038</t>
+    <t>3.8118</t>
+  </si>
+  <si>
+    <t>0.60645</t>
+  </si>
+  <si>
+    <t>0.090673</t>
+  </si>
+  <si>
+    <t>0.49113</t>
+  </si>
+  <si>
+    <t>0.012718</t>
+  </si>
+  <si>
+    <t>4.7935</t>
+  </si>
+  <si>
+    <t>1312.6953</t>
+  </si>
+  <si>
+    <t>538.5986</t>
   </si>
   <si>
     <t>Fluo-C2DL-MSC</t>
   </si>
   <si>
-    <t>54.4135</t>
-  </si>
-  <si>
-    <t>2.3256</t>
-  </si>
-  <si>
-    <t>0.93785</t>
-  </si>
-  <si>
-    <t>0.0067775</t>
-  </si>
-  <si>
-    <t>0.24414</t>
-  </si>
-  <si>
-    <t>0.065849</t>
-  </si>
-  <si>
-    <t>8.8942</t>
-  </si>
-  <si>
-    <t>389.3162</t>
-  </si>
-  <si>
-    <t>204.0334</t>
+    <t>77.4937</t>
+  </si>
+  <si>
+    <t>1.813</t>
+  </si>
+  <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>0.0077078</t>
+  </si>
+  <si>
+    <t>0.162</t>
+  </si>
+  <si>
+    <t>0.036557</t>
+  </si>
+  <si>
+    <t>9.1488</t>
+  </si>
+  <si>
+    <t>982.9109</t>
+  </si>
+  <si>
+    <t>92.12</t>
   </si>
   <si>
     <t>Fluo-C3DH-A549</t>
   </si>
   <si>
-    <t>9.7343</t>
-  </si>
-  <si>
-    <t>5.2647</t>
-  </si>
-  <si>
-    <t>0.80853</t>
-  </si>
-  <si>
-    <t>0.01183</t>
-  </si>
-  <si>
-    <t>0.048124</t>
-  </si>
-  <si>
-    <t>2.4</t>
-  </si>
-  <si>
-    <t>15040.7599</t>
+    <t>8.7793</t>
+  </si>
+  <si>
+    <t>5.6657</t>
+  </si>
+  <si>
+    <t>0.0084438</t>
+  </si>
+  <si>
+    <t>0.31375</t>
+  </si>
+  <si>
+    <t>0.041513</t>
+  </si>
+  <si>
+    <t>2.5953</t>
+  </si>
+  <si>
+    <t>418.2789</t>
   </si>
   <si>
     <t>Fluo-C3DH-H157</t>
   </si>
   <si>
-    <t>17.5617</t>
-  </si>
-  <si>
-    <t>5.6523</t>
-  </si>
-  <si>
-    <t>0.75</t>
-  </si>
-  <si>
-    <t>0.0098275</t>
-  </si>
-  <si>
-    <t>0.5255</t>
-  </si>
-  <si>
-    <t>0.062537</t>
-  </si>
-  <si>
-    <t>8.458</t>
-  </si>
-  <si>
-    <t>903.7605</t>
-  </si>
-  <si>
-    <t>80.5034</t>
+    <t>53.0769</t>
+  </si>
+  <si>
+    <t>3.5459</t>
+  </si>
+  <si>
+    <t>0.65646</t>
+  </si>
+  <si>
+    <t>0.0054233</t>
+  </si>
+  <si>
+    <t>0.18139</t>
+  </si>
+  <si>
+    <t>0.023539</t>
+  </si>
+  <si>
+    <t>8.6047</t>
+  </si>
+  <si>
+    <t>39378.0306</t>
+  </si>
+  <si>
+    <t>18.5026</t>
   </si>
   <si>
     <t>Fluo-C3DL-MDA231</t>
   </si>
   <si>
-    <t>11.682</t>
-  </si>
-  <si>
-    <t>1.0248</t>
-  </si>
-  <si>
-    <t>1.0548</t>
-  </si>
-  <si>
-    <t>0.019194</t>
-  </si>
-  <si>
-    <t>0.162</t>
-  </si>
-  <si>
-    <t>0.024532</t>
-  </si>
-  <si>
-    <t>1.2132</t>
-  </si>
-  <si>
-    <t>371.8122</t>
-  </si>
-  <si>
-    <t>21.3189</t>
+    <t>19.8992</t>
+  </si>
+  <si>
+    <t>1.5631</t>
+  </si>
+  <si>
+    <t>1.2894</t>
+  </si>
+  <si>
+    <t>0.021601</t>
+  </si>
+  <si>
+    <t>0.034126</t>
+  </si>
+  <si>
+    <t>1.2975</t>
+  </si>
+  <si>
+    <t>179.6401</t>
+  </si>
+  <si>
+    <t>18.1128</t>
   </si>
   <si>
     <t>Fluo-N2DH-GOWT1</t>
   </si>
   <si>
-    <t>18.9094</t>
-  </si>
-  <si>
-    <t>1.0587</t>
-  </si>
-  <si>
-    <t>0.71777</t>
-  </si>
-  <si>
-    <t>0.0033783</t>
-  </si>
-  <si>
-    <t>0.29754</t>
-  </si>
-  <si>
-    <t>13.1177</t>
-  </si>
-  <si>
-    <t>445.3405</t>
-  </si>
-  <si>
-    <t>14.4299</t>
+    <t>17.7822</t>
+  </si>
+  <si>
+    <t>1.0852</t>
+  </si>
+  <si>
+    <t>0.81</t>
+  </si>
+  <si>
+    <t>0.0025585</t>
+  </si>
+  <si>
+    <t>0.17621</t>
+  </si>
+  <si>
+    <t>0.1867</t>
+  </si>
+  <si>
+    <t>12.2929</t>
+  </si>
+  <si>
+    <t>421.8607</t>
+  </si>
+  <si>
+    <t>18.3432</t>
   </si>
   <si>
     <t>Fluo-N2DL-HeLa</t>
   </si>
   <si>
-    <t>7.1848</t>
-  </si>
-  <si>
-    <t>0.3026</t>
-  </si>
-  <si>
-    <t>0.38021</t>
-  </si>
-  <si>
-    <t>0.0013801</t>
-  </si>
-  <si>
-    <t>0.031968</t>
-  </si>
-  <si>
-    <t>0.6563</t>
-  </si>
-  <si>
-    <t>71.3406</t>
+    <t>6.9982</t>
+  </si>
+  <si>
+    <t>0.71903</t>
+  </si>
+  <si>
+    <t>0.70765</t>
+  </si>
+  <si>
+    <t>0.0066441</t>
+  </si>
+  <si>
+    <t>0.26729</t>
+  </si>
+  <si>
+    <t>0.11889</t>
+  </si>
+  <si>
+    <t>0.79866</t>
+  </si>
+  <si>
+    <t>68.5305</t>
+  </si>
+  <si>
+    <t>2.8283</t>
   </si>
   <si>
     <t>Fluo-N3DH-CE</t>
   </si>
   <si>
-    <t>14.285</t>
-  </si>
-  <si>
-    <t>7.1596</t>
-  </si>
-  <si>
-    <t>0.95</t>
-  </si>
-  <si>
-    <t>0.01016</t>
-  </si>
-  <si>
-    <t>0.45</t>
-  </si>
-  <si>
-    <t>0.024111</t>
-  </si>
-  <si>
-    <t>1.9463</t>
-  </si>
-  <si>
-    <t>2748.2639</t>
-  </si>
-  <si>
-    <t>712.8348</t>
+    <t>16.2215</t>
+  </si>
+  <si>
+    <t>5.8692</t>
+  </si>
+  <si>
+    <t>0.92416</t>
+  </si>
+  <si>
+    <t>0.020546</t>
+  </si>
+  <si>
+    <t>0.84693</t>
+  </si>
+  <si>
+    <t>0.021289</t>
+  </si>
+  <si>
+    <t>2.1391</t>
+  </si>
+  <si>
+    <t>1215.6487</t>
+  </si>
+  <si>
+    <t>245.4895</t>
   </si>
   <si>
     <t>Fluo-N3DH-CHO</t>
   </si>
   <si>
-    <t>10.8586</t>
-  </si>
-  <si>
-    <t>3.4507</t>
-  </si>
-  <si>
-    <t>0.4512</t>
-  </si>
-  <si>
-    <t>0.027725</t>
-  </si>
-  <si>
-    <t>0.09</t>
-  </si>
-  <si>
-    <t>0.0058462</t>
-  </si>
-  <si>
-    <t>5.607</t>
-  </si>
-  <si>
-    <t>6461.7219</t>
-  </si>
-  <si>
-    <t>433.9042</t>
+    <t>32.2599</t>
+  </si>
+  <si>
+    <t>0.82942</t>
+  </si>
+  <si>
+    <t>0.81103</t>
+  </si>
+  <si>
+    <t>0.021175</t>
+  </si>
+  <si>
+    <t>0.11647</t>
+  </si>
+  <si>
+    <t>0.013565</t>
+  </si>
+  <si>
+    <t>10.2495</t>
+  </si>
+  <si>
+    <t>5257.9213</t>
+  </si>
+  <si>
+    <t>424.6661</t>
   </si>
   <si>
     <t>PhC-C2DH-U373</t>
   </si>
   <si>
-    <t>17.8257</t>
-  </si>
-  <si>
-    <t>5.0664</t>
-  </si>
-  <si>
-    <t>0.87225</t>
-  </si>
-  <si>
-    <t>0.0061385</t>
-  </si>
-  <si>
-    <t>0.025132</t>
-  </si>
-  <si>
-    <t>6.7845</t>
-  </si>
-  <si>
-    <t>344.1373</t>
+    <t>13.234</t>
+  </si>
+  <si>
+    <t>4.5394</t>
+  </si>
+  <si>
+    <t>0.92221</t>
+  </si>
+  <si>
+    <t>0.0001266</t>
+  </si>
+  <si>
+    <t>0.89248</t>
+  </si>
+  <si>
+    <t>0.02551</t>
+  </si>
+  <si>
+    <t>6.0726</t>
+  </si>
+  <si>
+    <t>759.879</t>
+  </si>
+  <si>
+    <t>290.0805</t>
   </si>
   <si>
     <t>PhC-C2DL-PSC</t>
   </si>
   <si>
-    <t>4.4189</t>
-  </si>
-  <si>
-    <t>1.674</t>
-  </si>
-  <si>
-    <t>0.0055322</t>
-  </si>
-  <si>
-    <t>0.90563</t>
-  </si>
-  <si>
-    <t>0.035146</t>
-  </si>
-  <si>
-    <t>2.3188</t>
-  </si>
-  <si>
-    <t>33.9887</t>
+    <t>4.5266</t>
+  </si>
+  <si>
+    <t>1.2743</t>
+  </si>
+  <si>
+    <t>0.0052341</t>
+  </si>
+  <si>
+    <t>0.89937</t>
+  </si>
+  <si>
+    <t>0.03421</t>
+  </si>
+  <si>
+    <t>1.0144</t>
+  </si>
+  <si>
+    <t>29.7931</t>
+  </si>
+  <si>
+    <t>21.0108</t>
   </si>
 </sst>
 </file>
@@ -1341,116 +1362,116 @@
       <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="E3">
-        <v>0</v>
+      <c r="E3" t="s">
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3">
-        <v>191</v>
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J6">
         <v>5</v>
@@ -1458,258 +1479,258 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="F9" t="s">
+        <v>81</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="F10" t="s">
+        <v>91</v>
       </c>
       <c r="G10" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H10" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="I10" t="s">
-        <v>91</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
+        <v>94</v>
+      </c>
+      <c r="J10" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D11" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F11" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G11" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="H11" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="I11" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="J11" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E12" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F12" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G12" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H12" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="I12" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="J12" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D13" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E13" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="F13" t="s">
+        <v>121</v>
       </c>
       <c r="G13" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="H13" t="s">
-        <v>118</v>
-      </c>
-      <c r="I13">
+        <v>123</v>
+      </c>
+      <c r="I13" t="s">
+        <v>124</v>
+      </c>
+      <c r="J13" t="s">
         <v>125</v>
-      </c>
-      <c r="J13" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F14" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="G14" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="H14" t="s">
-        <v>126</v>
-      </c>
-      <c r="I14">
-        <v>45</v>
+        <v>132</v>
+      </c>
+      <c r="I14" t="s">
+        <v>133</v>
       </c>
       <c r="J14" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>